<commit_message>
streaming: LED button control filters
</commit_message>
<xml_diff>
--- a/results/streaming_noise.xlsx
+++ b/results/streaming_noise.xlsx
@@ -412,7 +412,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:J38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F13" sqref="F13"/>
@@ -488,6 +488,393 @@
         <v>5</v>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>0</v>
+      </c>
+      <c r="C14" t="n">
+        <v>9</v>
+      </c>
+      <c r="D14" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>7</v>
+      </c>
+      <c r="C17" t="n">
+        <v>5</v>
+      </c>
+      <c r="D17" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>1</v>
+      </c>
+      <c r="C18" t="n">
+        <v>17</v>
+      </c>
+      <c r="D18" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>test1</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>test1</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>12</v>
+      </c>
+      <c r="C21" t="n">
+        <v>0</v>
+      </c>
+      <c r="D21" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>test1</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>15</v>
+      </c>
+      <c r="C22" t="n">
+        <v>3</v>
+      </c>
+      <c r="D22" t="n">
+        <v>6</v>
+      </c>
+      <c r="E22" t="n">
+        <v>4</v>
+      </c>
+      <c r="F22" t="n">
+        <v>14</v>
+      </c>
+      <c r="G22" t="n">
+        <v>4</v>
+      </c>
+      <c r="H22" t="n">
+        <v>0</v>
+      </c>
+      <c r="I22" t="n">
+        <v>18</v>
+      </c>
+      <c r="J22" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>test1</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>test1</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>test1</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>test1</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>test1</t>
+        </is>
+      </c>
+      <c r="B27" t="n">
+        <v>2</v>
+      </c>
+      <c r="C27" t="n">
+        <v>18</v>
+      </c>
+      <c r="D27" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>test1</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>test1</t>
+        </is>
+      </c>
+      <c r="B29" t="n">
+        <v>1</v>
+      </c>
+      <c r="C29" t="n">
+        <v>19</v>
+      </c>
+      <c r="D29" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>test1</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>test1</t>
+        </is>
+      </c>
+      <c r="B31" t="n">
+        <v>2</v>
+      </c>
+      <c r="C31" t="n">
+        <v>18</v>
+      </c>
+      <c r="D31" t="n">
+        <v>0</v>
+      </c>
+      <c r="E31" t="n">
+        <v>0</v>
+      </c>
+      <c r="F31" t="n">
+        <v>20</v>
+      </c>
+      <c r="G31" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>test1</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>test1</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>test1</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>test1</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>test1</t>
+        </is>
+      </c>
+      <c r="B36" t="n">
+        <v>3</v>
+      </c>
+      <c r="C36" t="n">
+        <v>17</v>
+      </c>
+      <c r="D36" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>test1</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>test1</t>
+        </is>
+      </c>
+      <c r="B38" t="n">
+        <v>11</v>
+      </c>
+      <c r="C38" t="n">
+        <v>9</v>
+      </c>
+      <c r="D38" t="n">
+        <v>0</v>
+      </c>
+      <c r="E38" t="n">
+        <v>11</v>
+      </c>
+      <c r="F38" t="n">
+        <v>9</v>
+      </c>
+      <c r="G38" t="n">
+        <v>0</v>
+      </c>
+      <c r="H38" t="n">
+        <v>16</v>
+      </c>
+      <c r="I38" t="n">
+        <v>4</v>
+      </c>
+      <c r="J38" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>